<commit_message>
switch automatiquement vers le décompte
</commit_message>
<xml_diff>
--- a/Sample/chronogramme.xlsx
+++ b/Sample/chronogramme.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julien.mousqueton@computacenter.com/Code/rempar/Sample/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73AE586D-0101-9549-8B53-E4C5E3C25891}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F22E8C2E-EC26-F347-AAF0-990B6989D9B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="20960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1649" uniqueCount="615">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1643" uniqueCount="612">
   <si>
     <t>id</t>
   </si>
@@ -1507,22 +1507,13 @@
     <t>Mise à jour de la situation en cours. #RH</t>
   </si>
   <si>
-    <t>Communication en préparation. #BD #securite #juridique</t>
-  </si>
-  <si>
     <t xml:space="preserve">Coordination avec les parties prenantes. </t>
   </si>
   <si>
     <t>Pouvez-vous préparer un résumé d’une page pour diffusion interne ? #securite</t>
   </si>
   <si>
-    <t>Analyse des journaux en cours. #IT</t>
-  </si>
-  <si>
     <t>Information au public à venir. #RGPD #IT #crise</t>
-  </si>
-  <si>
-    <t>Coordination avec les parties prenantes. #BD #SI</t>
   </si>
   <si>
     <t>Rétablissement progressif des services. #cloud #communication #prod</t>
@@ -2244,7 +2235,7 @@
   <dimension ref="A1:I261"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A108" workbookViewId="0">
-      <selection activeCell="F118" sqref="F118"/>
+      <selection activeCell="F127" sqref="F127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2303,10 +2294,10 @@
         <v>406</v>
       </c>
       <c r="G2" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="H2" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -2329,13 +2320,13 @@
         <v>407</v>
       </c>
       <c r="G3" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="H3" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="I3" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -2372,13 +2363,13 @@
         <v>409</v>
       </c>
       <c r="G5" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="H5" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="I5" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -2395,7 +2386,7 @@
         <v>410</v>
       </c>
       <c r="H6" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -2426,7 +2417,7 @@
         <v>412</v>
       </c>
       <c r="H8" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -2449,13 +2440,13 @@
         <v>413</v>
       </c>
       <c r="G9" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="H9" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="I9" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -2472,7 +2463,7 @@
         <v>414</v>
       </c>
       <c r="H10" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -2489,7 +2480,7 @@
         <v>415</v>
       </c>
       <c r="H11" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -2526,13 +2517,13 @@
         <v>406</v>
       </c>
       <c r="G13" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="H13" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="I13" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -2555,10 +2546,10 @@
         <v>417</v>
       </c>
       <c r="G14" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="H14" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -2581,13 +2572,13 @@
         <v>418</v>
       </c>
       <c r="G15" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="H15" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="I15" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
@@ -2604,7 +2595,7 @@
         <v>419</v>
       </c>
       <c r="H16" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
@@ -2627,13 +2618,13 @@
         <v>420</v>
       </c>
       <c r="G17" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="H17" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="I17" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
@@ -2670,10 +2661,10 @@
         <v>422</v>
       </c>
       <c r="G19" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="H19" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
@@ -2710,13 +2701,13 @@
         <v>406</v>
       </c>
       <c r="G21" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="H21" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="I21" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
@@ -2739,13 +2730,13 @@
         <v>424</v>
       </c>
       <c r="G22" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="H22" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="I22" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
@@ -2768,13 +2759,13 @@
         <v>425</v>
       </c>
       <c r="G23" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="H23" t="s">
+        <v>607</v>
+      </c>
+      <c r="I23" t="s">
         <v>610</v>
-      </c>
-      <c r="I23" t="s">
-        <v>613</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
@@ -2867,13 +2858,13 @@
         <v>424</v>
       </c>
       <c r="G29" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="H29" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="I29" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
@@ -2910,13 +2901,13 @@
         <v>432</v>
       </c>
       <c r="G31" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="H31" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="I31" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
@@ -2939,13 +2930,13 @@
         <v>418</v>
       </c>
       <c r="G32" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="H32" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="I32" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
@@ -2996,13 +2987,13 @@
         <v>435</v>
       </c>
       <c r="G35" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="H35" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="I35" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
@@ -3033,7 +3024,7 @@
         <v>437</v>
       </c>
       <c r="H37" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
@@ -3070,10 +3061,10 @@
         <v>420</v>
       </c>
       <c r="G39" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="H39" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
@@ -3096,10 +3087,10 @@
         <v>424</v>
       </c>
       <c r="G40" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="H40" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
@@ -3122,13 +3113,13 @@
         <v>439</v>
       </c>
       <c r="G41" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="H41" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="I41" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
@@ -3159,7 +3150,7 @@
         <v>440</v>
       </c>
       <c r="H43" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
@@ -3210,13 +3201,13 @@
         <v>406</v>
       </c>
       <c r="G46" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="H46" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="I46" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
@@ -3239,10 +3230,10 @@
         <v>417</v>
       </c>
       <c r="G47" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="H47" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
@@ -3329,7 +3320,7 @@
         <v>446</v>
       </c>
       <c r="H53" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
@@ -3366,13 +3357,13 @@
         <v>422</v>
       </c>
       <c r="G55" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="H55" t="s">
+        <v>606</v>
+      </c>
+      <c r="I55" t="s">
         <v>609</v>
-      </c>
-      <c r="I55" t="s">
-        <v>612</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
@@ -3395,13 +3386,13 @@
         <v>448</v>
       </c>
       <c r="G56" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="H56" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="I56" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
@@ -3424,13 +3415,13 @@
         <v>418</v>
       </c>
       <c r="G57" t="s">
+        <v>598</v>
+      </c>
+      <c r="H57" t="s">
         <v>601</v>
       </c>
-      <c r="H57" t="s">
-        <v>604</v>
-      </c>
       <c r="I57" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
@@ -3453,13 +3444,13 @@
         <v>449</v>
       </c>
       <c r="G58" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="H58" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="I58" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
@@ -3496,13 +3487,13 @@
         <v>406</v>
       </c>
       <c r="G60" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="H60" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="I60" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
@@ -3553,13 +3544,13 @@
         <v>417</v>
       </c>
       <c r="G63" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="H63" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="I63" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.2">
@@ -3582,13 +3573,13 @@
         <v>424</v>
       </c>
       <c r="G64" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="H64" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="I64" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.2">
@@ -3611,13 +3602,13 @@
         <v>453</v>
       </c>
       <c r="G65" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="H65" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="I65" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.2">
@@ -3648,7 +3639,7 @@
         <v>455</v>
       </c>
       <c r="H67" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.2">
@@ -3665,7 +3656,7 @@
         <v>456</v>
       </c>
       <c r="H68" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
@@ -3702,13 +3693,13 @@
         <v>458</v>
       </c>
       <c r="G70" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="H70" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="I70" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.2">
@@ -3745,13 +3736,13 @@
         <v>460</v>
       </c>
       <c r="G72" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="H72" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="I72" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.2">
@@ -3782,7 +3773,7 @@
         <v>461</v>
       </c>
       <c r="H74" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.2">
@@ -3805,10 +3796,10 @@
         <v>462</v>
       </c>
       <c r="G75" t="s">
+        <v>600</v>
+      </c>
+      <c r="H75" t="s">
         <v>603</v>
-      </c>
-      <c r="H75" t="s">
-        <v>606</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.2">
@@ -3831,10 +3822,10 @@
         <v>463</v>
       </c>
       <c r="G76" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="H76" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.2">
@@ -3871,13 +3862,13 @@
         <v>465</v>
       </c>
       <c r="G78" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="H78" t="s">
+        <v>607</v>
+      </c>
+      <c r="I78" t="s">
         <v>610</v>
-      </c>
-      <c r="I78" t="s">
-        <v>613</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.2">
@@ -3914,13 +3905,13 @@
         <v>422</v>
       </c>
       <c r="G80" t="s">
+        <v>598</v>
+      </c>
+      <c r="H80" t="s">
         <v>601</v>
       </c>
-      <c r="H80" t="s">
-        <v>604</v>
-      </c>
       <c r="I80" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.2">
@@ -3971,13 +3962,13 @@
         <v>468</v>
       </c>
       <c r="G83" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="H83" t="s">
+        <v>605</v>
+      </c>
+      <c r="I83" t="s">
         <v>608</v>
-      </c>
-      <c r="I83" t="s">
-        <v>611</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.2">
@@ -4000,10 +3991,10 @@
         <v>469</v>
       </c>
       <c r="G84" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="H84" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.2">
@@ -4040,13 +4031,13 @@
         <v>406</v>
       </c>
       <c r="G86" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="H86" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="I86" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.2">
@@ -4091,7 +4082,7 @@
         <v>473</v>
       </c>
       <c r="H89" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.2">
@@ -4114,13 +4105,13 @@
         <v>406</v>
       </c>
       <c r="G90" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="H90" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="I90" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.2">
@@ -4143,10 +4134,10 @@
         <v>422</v>
       </c>
       <c r="G91" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="H91" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.2">
@@ -4169,13 +4160,13 @@
         <v>474</v>
       </c>
       <c r="G92" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="H92" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="I92" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.2">
@@ -4198,13 +4189,13 @@
         <v>420</v>
       </c>
       <c r="G93" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="H93" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="I93" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.2">
@@ -4241,13 +4232,13 @@
         <v>476</v>
       </c>
       <c r="G95" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="H95" t="s">
+        <v>607</v>
+      </c>
+      <c r="I95" t="s">
         <v>610</v>
-      </c>
-      <c r="I95" t="s">
-        <v>613</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.2">
@@ -4270,13 +4261,13 @@
         <v>477</v>
       </c>
       <c r="G96" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="H96" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="I96" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.2">
@@ -4293,7 +4284,7 @@
         <v>423</v>
       </c>
       <c r="H97" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.2">
@@ -4310,7 +4301,7 @@
         <v>478</v>
       </c>
       <c r="H98" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.2">
@@ -4347,10 +4338,10 @@
         <v>420</v>
       </c>
       <c r="G100" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="H100" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.2">
@@ -4387,13 +4378,13 @@
         <v>424</v>
       </c>
       <c r="G102" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="H102" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="I102" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.2">
@@ -4416,13 +4407,13 @@
         <v>481</v>
       </c>
       <c r="G103" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="H103" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="I103" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.2">
@@ -4445,10 +4436,10 @@
         <v>474</v>
       </c>
       <c r="G104" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="H104" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.2">
@@ -4471,13 +4462,13 @@
         <v>482</v>
       </c>
       <c r="G105" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="H105" t="s">
+        <v>607</v>
+      </c>
+      <c r="I105" t="s">
         <v>610</v>
-      </c>
-      <c r="I105" t="s">
-        <v>613</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.2">
@@ -4500,10 +4491,10 @@
         <v>483</v>
       </c>
       <c r="G106" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="H106" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.2">
@@ -4526,10 +4517,10 @@
         <v>484</v>
       </c>
       <c r="G107" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="H107" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.2">
@@ -4580,13 +4571,13 @@
         <v>474</v>
       </c>
       <c r="G110" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="H110" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="I110" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.2">
@@ -4651,13 +4642,13 @@
         <v>489</v>
       </c>
       <c r="G114" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="H114" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="I114" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.2">
@@ -4680,13 +4671,13 @@
         <v>490</v>
       </c>
       <c r="G115" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="H115" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="I115" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.2">
@@ -4703,7 +4694,7 @@
         <v>491</v>
       </c>
       <c r="H116" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.2">
@@ -4725,7 +4716,7 @@
         <v>243</v>
       </c>
       <c r="C118" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
       <c r="F118">
         <v>25</v>
@@ -4750,13 +4741,10 @@
         <v>245</v>
       </c>
       <c r="C120" t="s">
-        <v>388</v>
-      </c>
-      <c r="D120" t="s">
-        <v>389</v>
-      </c>
-      <c r="F120" t="s">
-        <v>494</v>
+        <v>611</v>
+      </c>
+      <c r="F120">
+        <v>5</v>
       </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.2">
@@ -4770,10 +4758,10 @@
         <v>394</v>
       </c>
       <c r="F121" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="H121" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.2">
@@ -4793,16 +4781,16 @@
         <v>402</v>
       </c>
       <c r="F122" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="G122" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="H122" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="I122" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.2">
@@ -4825,13 +4813,13 @@
         <v>420</v>
       </c>
       <c r="G123" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="H123" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="I123" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.2">
@@ -4839,13 +4827,10 @@
         <v>249</v>
       </c>
       <c r="C124" t="s">
-        <v>388</v>
-      </c>
-      <c r="D124" t="s">
-        <v>398</v>
-      </c>
-      <c r="F124" t="s">
-        <v>497</v>
+        <v>611</v>
+      </c>
+      <c r="F124">
+        <v>5</v>
       </c>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.2">
@@ -4859,7 +4844,7 @@
         <v>393</v>
       </c>
       <c r="F125" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.2">
@@ -4867,13 +4852,10 @@
         <v>251</v>
       </c>
       <c r="C126" t="s">
-        <v>388</v>
-      </c>
-      <c r="D126" t="s">
-        <v>391</v>
-      </c>
-      <c r="F126" t="s">
-        <v>499</v>
+        <v>611</v>
+      </c>
+      <c r="F126">
+        <v>5</v>
       </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.2">
@@ -4887,10 +4869,10 @@
         <v>399</v>
       </c>
       <c r="F127" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="H127" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.2">
@@ -4910,16 +4892,16 @@
         <v>400</v>
       </c>
       <c r="F128" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="G128" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="H128" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="I128" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.2">
@@ -4933,7 +4915,7 @@
         <v>393</v>
       </c>
       <c r="F129" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.2">
@@ -4953,16 +4935,16 @@
         <v>401</v>
       </c>
       <c r="F130" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="G130" t="s">
+        <v>599</v>
+      </c>
+      <c r="H130" t="s">
         <v>602</v>
       </c>
-      <c r="H130" t="s">
-        <v>605</v>
-      </c>
       <c r="I130" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.2">
@@ -4982,16 +4964,16 @@
         <v>404</v>
       </c>
       <c r="F131" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="G131" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="H131" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="I131" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.2">
@@ -5019,7 +5001,7 @@
         <v>396</v>
       </c>
       <c r="F133" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.2">
@@ -5033,10 +5015,10 @@
         <v>395</v>
       </c>
       <c r="F134" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="H134" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.2">
@@ -5056,16 +5038,16 @@
         <v>404</v>
       </c>
       <c r="F135" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="G135" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="H135" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="I135" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.2">
@@ -5079,7 +5061,7 @@
         <v>398</v>
       </c>
       <c r="F136" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.2">
@@ -5099,16 +5081,16 @@
         <v>405</v>
       </c>
       <c r="F137" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="G137" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="H137" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="I137" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.2">
@@ -5128,13 +5110,13 @@
         <v>404</v>
       </c>
       <c r="F138" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="G138" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="H138" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.2">
@@ -5157,13 +5139,13 @@
         <v>462</v>
       </c>
       <c r="G139" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="H139" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="I139" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.2">
@@ -5177,7 +5159,7 @@
         <v>394</v>
       </c>
       <c r="F140" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.2">
@@ -5197,16 +5179,16 @@
         <v>405</v>
       </c>
       <c r="F141" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="G141" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="H141" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="I141" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.2">
@@ -5220,7 +5202,7 @@
         <v>393</v>
       </c>
       <c r="F142" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.2">
@@ -5240,16 +5222,16 @@
         <v>403</v>
       </c>
       <c r="F143" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="G143" t="s">
+        <v>600</v>
+      </c>
+      <c r="H143" t="s">
         <v>603</v>
       </c>
-      <c r="H143" t="s">
-        <v>606</v>
-      </c>
       <c r="I143" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.2">
@@ -5277,10 +5259,10 @@
         <v>396</v>
       </c>
       <c r="F145" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="H145" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.2">
@@ -5300,13 +5282,13 @@
         <v>402</v>
       </c>
       <c r="F146" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="G146" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="H146" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.2">
@@ -5320,10 +5302,10 @@
         <v>394</v>
       </c>
       <c r="F147" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="H147" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.2">
@@ -5337,7 +5319,7 @@
         <v>390</v>
       </c>
       <c r="F148" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.2">
@@ -5351,10 +5333,10 @@
         <v>399</v>
       </c>
       <c r="F149" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="H149" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.2">
@@ -5377,10 +5359,10 @@
         <v>424</v>
       </c>
       <c r="G150" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="H150" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.2">
@@ -5394,7 +5376,7 @@
         <v>397</v>
       </c>
       <c r="F151" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.2">
@@ -5414,13 +5396,13 @@
         <v>403</v>
       </c>
       <c r="F152" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="G152" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="H152" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.2">
@@ -5440,16 +5422,16 @@
         <v>404</v>
       </c>
       <c r="F153" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="G153" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="H153" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="I153" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.2">
@@ -5469,16 +5451,16 @@
         <v>403</v>
       </c>
       <c r="F154" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="G154" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="H154" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="I154" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
     </row>
     <row r="155" spans="1:9" x14ac:dyDescent="0.2">
@@ -5492,10 +5474,10 @@
         <v>397</v>
       </c>
       <c r="F155" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="H155" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
     </row>
     <row r="156" spans="1:9" x14ac:dyDescent="0.2">
@@ -5515,16 +5497,16 @@
         <v>405</v>
       </c>
       <c r="F156" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="G156" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="H156" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="I156" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.2">
@@ -5544,16 +5526,16 @@
         <v>403</v>
       </c>
       <c r="F157" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="G157" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="H157" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="I157" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.2">
@@ -5581,7 +5563,7 @@
         <v>389</v>
       </c>
       <c r="F159" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.2">
@@ -5604,13 +5586,13 @@
         <v>417</v>
       </c>
       <c r="G160" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="H160" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="I160" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
     </row>
     <row r="161" spans="1:9" x14ac:dyDescent="0.2">
@@ -5633,13 +5615,13 @@
         <v>417</v>
       </c>
       <c r="G161" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="H161" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="I161" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
     </row>
     <row r="162" spans="1:9" x14ac:dyDescent="0.2">
@@ -5659,16 +5641,16 @@
         <v>400</v>
       </c>
       <c r="F162" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="G162" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="H162" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="I162" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
     </row>
     <row r="163" spans="1:9" x14ac:dyDescent="0.2">
@@ -5685,7 +5667,7 @@
         <v>455</v>
       </c>
       <c r="H163" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
     </row>
     <row r="164" spans="1:9" x14ac:dyDescent="0.2">
@@ -5708,13 +5690,13 @@
         <v>468</v>
       </c>
       <c r="G164" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="H164" t="s">
+        <v>607</v>
+      </c>
+      <c r="I164" t="s">
         <v>610</v>
-      </c>
-      <c r="I164" t="s">
-        <v>613</v>
       </c>
     </row>
     <row r="165" spans="1:9" x14ac:dyDescent="0.2">
@@ -5728,7 +5710,7 @@
         <v>396</v>
       </c>
       <c r="F165" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
     </row>
     <row r="166" spans="1:9" x14ac:dyDescent="0.2">
@@ -5756,7 +5738,7 @@
         <v>396</v>
       </c>
       <c r="F167" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
     </row>
     <row r="168" spans="1:9" x14ac:dyDescent="0.2">
@@ -5770,10 +5752,10 @@
         <v>391</v>
       </c>
       <c r="F168" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="H168" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
     </row>
     <row r="169" spans="1:9" x14ac:dyDescent="0.2">
@@ -5793,16 +5775,16 @@
         <v>405</v>
       </c>
       <c r="F169" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="G169" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="H169" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="I169" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
     </row>
     <row r="170" spans="1:9" x14ac:dyDescent="0.2">
@@ -5822,13 +5804,13 @@
         <v>405</v>
       </c>
       <c r="F170" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="G170" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="H170" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
     </row>
     <row r="171" spans="1:9" x14ac:dyDescent="0.2">
@@ -5842,10 +5824,10 @@
         <v>394</v>
       </c>
       <c r="F171" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="H171" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
     </row>
     <row r="172" spans="1:9" x14ac:dyDescent="0.2">
@@ -5859,7 +5841,7 @@
         <v>398</v>
       </c>
       <c r="F172" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
     </row>
     <row r="173" spans="1:9" x14ac:dyDescent="0.2">
@@ -5873,7 +5855,7 @@
         <v>393</v>
       </c>
       <c r="F173" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
     </row>
     <row r="174" spans="1:9" x14ac:dyDescent="0.2">
@@ -5896,13 +5878,13 @@
         <v>417</v>
       </c>
       <c r="G174" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="H174" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="I174" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
     </row>
     <row r="175" spans="1:9" x14ac:dyDescent="0.2">
@@ -5925,13 +5907,13 @@
         <v>424</v>
       </c>
       <c r="G175" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="H175" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="I175" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
     </row>
     <row r="176" spans="1:9" x14ac:dyDescent="0.2">
@@ -5951,13 +5933,13 @@
         <v>401</v>
       </c>
       <c r="F176" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="G176" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="H176" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
     </row>
     <row r="177" spans="1:9" x14ac:dyDescent="0.2">
@@ -5971,10 +5953,10 @@
         <v>393</v>
       </c>
       <c r="F177" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="H177" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
     </row>
     <row r="178" spans="1:9" x14ac:dyDescent="0.2">
@@ -5988,7 +5970,7 @@
         <v>391</v>
       </c>
       <c r="F178" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
     </row>
     <row r="179" spans="1:9" x14ac:dyDescent="0.2">
@@ -6008,16 +5990,16 @@
         <v>401</v>
       </c>
       <c r="F179" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="G179" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="H179" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="I179" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
     </row>
     <row r="180" spans="1:9" x14ac:dyDescent="0.2">
@@ -6051,16 +6033,16 @@
         <v>404</v>
       </c>
       <c r="F181" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="G181" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="H181" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="I181" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
     </row>
     <row r="182" spans="1:9" x14ac:dyDescent="0.2">
@@ -6080,16 +6062,16 @@
         <v>401</v>
       </c>
       <c r="F182" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="G182" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="H182" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="I182" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
     </row>
     <row r="183" spans="1:9" x14ac:dyDescent="0.2">
@@ -6112,10 +6094,10 @@
         <v>422</v>
       </c>
       <c r="G183" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="H183" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
     </row>
     <row r="184" spans="1:9" x14ac:dyDescent="0.2">
@@ -6129,7 +6111,7 @@
         <v>392</v>
       </c>
       <c r="F184" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
     </row>
     <row r="185" spans="1:9" x14ac:dyDescent="0.2">
@@ -6143,7 +6125,7 @@
         <v>390</v>
       </c>
       <c r="F185" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
     </row>
     <row r="186" spans="1:9" x14ac:dyDescent="0.2">
@@ -6157,7 +6139,7 @@
         <v>390</v>
       </c>
       <c r="F186" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
     </row>
     <row r="187" spans="1:9" x14ac:dyDescent="0.2">
@@ -6180,13 +6162,13 @@
         <v>418</v>
       </c>
       <c r="G187" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="H187" t="s">
+        <v>606</v>
+      </c>
+      <c r="I187" t="s">
         <v>609</v>
-      </c>
-      <c r="I187" t="s">
-        <v>612</v>
       </c>
     </row>
     <row r="188" spans="1:9" x14ac:dyDescent="0.2">
@@ -6200,7 +6182,7 @@
         <v>396</v>
       </c>
       <c r="F188" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
     </row>
     <row r="189" spans="1:9" x14ac:dyDescent="0.2">
@@ -6220,16 +6202,16 @@
         <v>401</v>
       </c>
       <c r="F189" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="G189" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="H189" t="s">
+        <v>607</v>
+      </c>
+      <c r="I189" t="s">
         <v>610</v>
-      </c>
-      <c r="I189" t="s">
-        <v>613</v>
       </c>
     </row>
     <row r="190" spans="1:9" x14ac:dyDescent="0.2">
@@ -6243,10 +6225,10 @@
         <v>397</v>
       </c>
       <c r="F190" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
       <c r="H190" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
     </row>
     <row r="191" spans="1:9" x14ac:dyDescent="0.2">
@@ -6269,13 +6251,13 @@
         <v>406</v>
       </c>
       <c r="G191" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="H191" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="I191" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
     </row>
     <row r="192" spans="1:9" x14ac:dyDescent="0.2">
@@ -6295,16 +6277,16 @@
         <v>402</v>
       </c>
       <c r="F192" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="G192" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="H192" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="I192" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
     </row>
     <row r="193" spans="1:9" x14ac:dyDescent="0.2">
@@ -6318,7 +6300,7 @@
         <v>392</v>
       </c>
       <c r="F193" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
     </row>
     <row r="194" spans="1:9" x14ac:dyDescent="0.2">
@@ -6346,7 +6328,7 @@
         <v>390</v>
       </c>
       <c r="F195" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
     </row>
     <row r="196" spans="1:9" x14ac:dyDescent="0.2">
@@ -6366,16 +6348,16 @@
         <v>402</v>
       </c>
       <c r="F196" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="G196" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="H196" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="I196" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
     </row>
     <row r="197" spans="1:9" x14ac:dyDescent="0.2">
@@ -6389,10 +6371,10 @@
         <v>390</v>
       </c>
       <c r="F197" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="H197" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
     </row>
     <row r="198" spans="1:9" x14ac:dyDescent="0.2">
@@ -6415,13 +6397,13 @@
         <v>420</v>
       </c>
       <c r="G198" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="H198" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="I198" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
     </row>
     <row r="199" spans="1:9" x14ac:dyDescent="0.2">
@@ -6441,16 +6423,16 @@
         <v>403</v>
       </c>
       <c r="F199" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="G199" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="H199" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="I199" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
     </row>
     <row r="200" spans="1:9" x14ac:dyDescent="0.2">
@@ -6467,7 +6449,7 @@
         <v>447</v>
       </c>
       <c r="H200" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
     </row>
     <row r="201" spans="1:9" x14ac:dyDescent="0.2">
@@ -6481,7 +6463,7 @@
         <v>392</v>
       </c>
       <c r="F201" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
     </row>
     <row r="202" spans="1:9" x14ac:dyDescent="0.2">
@@ -6495,7 +6477,7 @@
         <v>398</v>
       </c>
       <c r="F202" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
     </row>
     <row r="203" spans="1:9" x14ac:dyDescent="0.2">
@@ -6529,16 +6511,16 @@
         <v>401</v>
       </c>
       <c r="F204" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="G204" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="H204" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="I204" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
     </row>
     <row r="205" spans="1:9" x14ac:dyDescent="0.2">
@@ -6558,13 +6540,13 @@
         <v>405</v>
       </c>
       <c r="F205" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="G205" t="s">
+        <v>599</v>
+      </c>
+      <c r="H205" t="s">
         <v>602</v>
-      </c>
-      <c r="H205" t="s">
-        <v>605</v>
       </c>
     </row>
     <row r="206" spans="1:9" x14ac:dyDescent="0.2">
@@ -6587,13 +6569,13 @@
         <v>474</v>
       </c>
       <c r="G206" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="H206" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="I206" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
     </row>
     <row r="207" spans="1:9" x14ac:dyDescent="0.2">
@@ -6613,16 +6595,16 @@
         <v>402</v>
       </c>
       <c r="F207" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="G207" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="H207" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="I207" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
     </row>
     <row r="208" spans="1:9" x14ac:dyDescent="0.2">
@@ -6636,7 +6618,7 @@
         <v>395</v>
       </c>
       <c r="F208" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
     </row>
     <row r="209" spans="1:9" x14ac:dyDescent="0.2">
@@ -6650,7 +6632,7 @@
         <v>389</v>
       </c>
       <c r="F209" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
     </row>
     <row r="210" spans="1:9" x14ac:dyDescent="0.2">
@@ -6670,16 +6652,16 @@
         <v>404</v>
       </c>
       <c r="F210" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="G210" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="H210" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="I210" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
     </row>
     <row r="211" spans="1:9" x14ac:dyDescent="0.2">
@@ -6702,13 +6684,13 @@
         <v>424</v>
       </c>
       <c r="G211" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="H211" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="I211" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
     </row>
     <row r="212" spans="1:9" x14ac:dyDescent="0.2">
@@ -6731,13 +6713,13 @@
         <v>418</v>
       </c>
       <c r="G212" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="H212" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="I212" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
     </row>
     <row r="213" spans="1:9" x14ac:dyDescent="0.2">
@@ -6751,7 +6733,7 @@
         <v>390</v>
       </c>
       <c r="F213" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
     </row>
     <row r="214" spans="1:9" x14ac:dyDescent="0.2">
@@ -6774,10 +6756,10 @@
         <v>422</v>
       </c>
       <c r="G214" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="H214" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
     </row>
     <row r="215" spans="1:9" x14ac:dyDescent="0.2">
@@ -6791,7 +6773,7 @@
         <v>393</v>
       </c>
       <c r="F215" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
     </row>
     <row r="216" spans="1:9" x14ac:dyDescent="0.2">
@@ -6805,10 +6787,10 @@
         <v>399</v>
       </c>
       <c r="F216" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="H216" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
     </row>
     <row r="217" spans="1:9" x14ac:dyDescent="0.2">
@@ -6822,7 +6804,7 @@
         <v>392</v>
       </c>
       <c r="F217" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
     </row>
     <row r="218" spans="1:9" x14ac:dyDescent="0.2">
@@ -6836,10 +6818,10 @@
         <v>390</v>
       </c>
       <c r="F218" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="H218" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
     </row>
     <row r="219" spans="1:9" x14ac:dyDescent="0.2">
@@ -6853,7 +6835,7 @@
         <v>397</v>
       </c>
       <c r="F219" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
     </row>
     <row r="220" spans="1:9" x14ac:dyDescent="0.2">
@@ -6867,7 +6849,7 @@
         <v>399</v>
       </c>
       <c r="F220" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
     </row>
     <row r="221" spans="1:9" x14ac:dyDescent="0.2">
@@ -6887,16 +6869,16 @@
         <v>403</v>
       </c>
       <c r="F221" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="G221" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="H221" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="I221" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
     </row>
     <row r="222" spans="1:9" x14ac:dyDescent="0.2">
@@ -6919,13 +6901,13 @@
         <v>422</v>
       </c>
       <c r="G222" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="H222" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="I222" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
     </row>
     <row r="223" spans="1:9" x14ac:dyDescent="0.2">
@@ -6948,13 +6930,13 @@
         <v>422</v>
       </c>
       <c r="G223" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="H223" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="I223" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
     </row>
     <row r="224" spans="1:9" x14ac:dyDescent="0.2">
@@ -6974,16 +6956,16 @@
         <v>400</v>
       </c>
       <c r="F224" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="G224" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="H224" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="I224" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
     </row>
     <row r="225" spans="1:9" x14ac:dyDescent="0.2">
@@ -7003,16 +6985,16 @@
         <v>400</v>
       </c>
       <c r="F225" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="G225" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="H225" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="I225" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
     </row>
     <row r="226" spans="1:9" x14ac:dyDescent="0.2">
@@ -7026,7 +7008,7 @@
         <v>398</v>
       </c>
       <c r="F226" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
     </row>
     <row r="227" spans="1:9" x14ac:dyDescent="0.2">
@@ -7046,16 +7028,16 @@
         <v>401</v>
       </c>
       <c r="F227" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="G227" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="H227" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="I227" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
     </row>
     <row r="228" spans="1:9" x14ac:dyDescent="0.2">
@@ -7086,7 +7068,7 @@
         <v>419</v>
       </c>
       <c r="H229" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
     </row>
     <row r="230" spans="1:9" x14ac:dyDescent="0.2">
@@ -7103,7 +7085,7 @@
         <v>455</v>
       </c>
       <c r="H230" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
     </row>
     <row r="231" spans="1:9" x14ac:dyDescent="0.2">
@@ -7123,16 +7105,16 @@
         <v>401</v>
       </c>
       <c r="F231" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="G231" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="H231" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="I231" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
     </row>
     <row r="232" spans="1:9" x14ac:dyDescent="0.2">
@@ -7155,10 +7137,10 @@
         <v>418</v>
       </c>
       <c r="G232" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="H232" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
     </row>
     <row r="233" spans="1:9" x14ac:dyDescent="0.2">
@@ -7181,13 +7163,13 @@
         <v>432</v>
       </c>
       <c r="G233" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="H233" t="s">
+        <v>605</v>
+      </c>
+      <c r="I233" t="s">
         <v>608</v>
-      </c>
-      <c r="I233" t="s">
-        <v>611</v>
       </c>
     </row>
     <row r="234" spans="1:9" x14ac:dyDescent="0.2">
@@ -7201,7 +7183,7 @@
         <v>394</v>
       </c>
       <c r="F234" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
     </row>
     <row r="235" spans="1:9" x14ac:dyDescent="0.2">
@@ -7215,7 +7197,7 @@
         <v>389</v>
       </c>
       <c r="F235" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
     </row>
     <row r="236" spans="1:9" x14ac:dyDescent="0.2">
@@ -7238,13 +7220,13 @@
         <v>422</v>
       </c>
       <c r="G236" t="s">
+        <v>599</v>
+      </c>
+      <c r="H236" t="s">
         <v>602</v>
       </c>
-      <c r="H236" t="s">
-        <v>605</v>
-      </c>
       <c r="I236" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
     </row>
     <row r="237" spans="1:9" x14ac:dyDescent="0.2">
@@ -7258,7 +7240,7 @@
         <v>398</v>
       </c>
       <c r="F237" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
     </row>
     <row r="238" spans="1:9" x14ac:dyDescent="0.2">
@@ -7278,16 +7260,16 @@
         <v>402</v>
       </c>
       <c r="F238" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="G238" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="H238" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="I238" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
     </row>
     <row r="239" spans="1:9" x14ac:dyDescent="0.2">
@@ -7301,7 +7283,7 @@
         <v>391</v>
       </c>
       <c r="F239" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
     </row>
     <row r="240" spans="1:9" x14ac:dyDescent="0.2">
@@ -7315,7 +7297,7 @@
         <v>399</v>
       </c>
       <c r="F240" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
     </row>
     <row r="241" spans="1:9" x14ac:dyDescent="0.2">
@@ -7343,7 +7325,7 @@
         <v>394</v>
       </c>
       <c r="F242" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
     </row>
     <row r="243" spans="1:9" x14ac:dyDescent="0.2">
@@ -7357,7 +7339,7 @@
         <v>397</v>
       </c>
       <c r="F243" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
     </row>
     <row r="244" spans="1:9" x14ac:dyDescent="0.2">
@@ -7371,7 +7353,7 @@
         <v>399</v>
       </c>
       <c r="F244" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
     </row>
     <row r="245" spans="1:9" x14ac:dyDescent="0.2">
@@ -7385,7 +7367,7 @@
         <v>394</v>
       </c>
       <c r="F245" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
     </row>
     <row r="246" spans="1:9" x14ac:dyDescent="0.2">
@@ -7405,16 +7387,16 @@
         <v>401</v>
       </c>
       <c r="F246" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="G246" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="H246" t="s">
+        <v>605</v>
+      </c>
+      <c r="I246" t="s">
         <v>608</v>
-      </c>
-      <c r="I246" t="s">
-        <v>611</v>
       </c>
     </row>
     <row r="247" spans="1:9" x14ac:dyDescent="0.2">
@@ -7437,13 +7419,13 @@
         <v>418</v>
       </c>
       <c r="G247" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="H247" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="I247" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
     </row>
     <row r="248" spans="1:9" x14ac:dyDescent="0.2">
@@ -7471,7 +7453,7 @@
         <v>396</v>
       </c>
       <c r="F249" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
     </row>
     <row r="250" spans="1:9" x14ac:dyDescent="0.2">
@@ -7485,7 +7467,7 @@
         <v>393</v>
       </c>
       <c r="F250" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
     </row>
     <row r="251" spans="1:9" x14ac:dyDescent="0.2">
@@ -7499,10 +7481,10 @@
         <v>393</v>
       </c>
       <c r="F251" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="H251" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
     </row>
     <row r="252" spans="1:9" x14ac:dyDescent="0.2">
@@ -7522,16 +7504,16 @@
         <v>404</v>
       </c>
       <c r="F252" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="G252" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="H252" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="I252" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
     </row>
     <row r="253" spans="1:9" x14ac:dyDescent="0.2">
@@ -7545,10 +7527,10 @@
         <v>399</v>
       </c>
       <c r="F253" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="H253" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
     </row>
     <row r="254" spans="1:9" x14ac:dyDescent="0.2">
@@ -7571,13 +7553,13 @@
         <v>406</v>
       </c>
       <c r="G254" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="H254" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="I254" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
     </row>
     <row r="255" spans="1:9" x14ac:dyDescent="0.2">
@@ -7591,7 +7573,7 @@
         <v>399</v>
       </c>
       <c r="F255" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
     </row>
     <row r="256" spans="1:9" x14ac:dyDescent="0.2">
@@ -7611,16 +7593,16 @@
         <v>400</v>
       </c>
       <c r="F256" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="G256" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="H256" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="I256" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
     </row>
     <row r="257" spans="1:9" x14ac:dyDescent="0.2">
@@ -7634,7 +7616,7 @@
         <v>398</v>
       </c>
       <c r="F257" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
     </row>
     <row r="258" spans="1:9" x14ac:dyDescent="0.2">
@@ -7651,7 +7633,7 @@
         <v>423</v>
       </c>
       <c r="H258" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
     </row>
     <row r="259" spans="1:9" x14ac:dyDescent="0.2">
@@ -7671,16 +7653,16 @@
         <v>400</v>
       </c>
       <c r="F259" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="G259" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="H259" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="I259" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
     </row>
     <row r="260" spans="1:9" x14ac:dyDescent="0.2">
@@ -7714,16 +7696,16 @@
         <v>405</v>
       </c>
       <c r="F261" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="G261" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="H261" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="I261" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
     </row>
   </sheetData>

</xml_diff>